<commit_message>
user sign in test case added
</commit_message>
<xml_diff>
--- a/Test case report for Dailyfinance.net.xlsx
+++ b/Test case report for Dailyfinance.net.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="242">
   <si>
     <t>Project Name:</t>
   </si>
@@ -766,6 +766,189 @@
 Phone Number: "01873195755"
 Address: "dhaka"
 </t>
+  </si>
+  <si>
+    <t>TC46</t>
+  </si>
+  <si>
+    <t>TC47</t>
+  </si>
+  <si>
+    <t>TC48</t>
+  </si>
+  <si>
+    <t>TC49</t>
+  </si>
+  <si>
+    <t>TC50</t>
+  </si>
+  <si>
+    <t>TC51</t>
+  </si>
+  <si>
+    <t>TC52</t>
+  </si>
+  <si>
+    <t>TC53</t>
+  </si>
+  <si>
+    <t>TC54</t>
+  </si>
+  <si>
+    <t>TC55</t>
+  </si>
+  <si>
+    <t>TC56</t>
+  </si>
+  <si>
+    <t>TC57</t>
+  </si>
+  <si>
+    <t>TC58</t>
+  </si>
+  <si>
+    <t>TC59</t>
+  </si>
+  <si>
+    <t>TC60</t>
+  </si>
+  <si>
+    <t>Sign In</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Go to https://dailyfinance.roadtocareer.net/
+</t>
+  </si>
+  <si>
+    <t>Keeping email and password field blank</t>
+  </si>
+  <si>
+    <t>Should not allow user to login and display an error messeage</t>
+  </si>
+  <si>
+    <t>Checking login wrong credentials in email and password field</t>
+  </si>
+  <si>
+    <t>Checking login wrong credentials in email field</t>
+  </si>
+  <si>
+    <t>Email: "testsofWizards@gmail.com"
+password: "wizard123"</t>
+  </si>
+  <si>
+    <t>Checking login wrong credentials in password field</t>
+  </si>
+  <si>
+    <t>Email: "testsofWizards@gmail.com"
+password: "wizard456"</t>
+  </si>
+  <si>
+    <t>Email: "testsofWizard@gmail.com"
+password: "wizard456"</t>
+  </si>
+  <si>
+    <t>Checking if the data in password is masked</t>
+  </si>
+  <si>
+    <t>password: "wizard123"</t>
+  </si>
+  <si>
+    <t>Should be masked</t>
+  </si>
+  <si>
+    <t>Checking login with valid credentials in email and password field</t>
+  </si>
+  <si>
+    <t>Email: "testsofWizard@gmail.com"
+password: "wizard123"</t>
+  </si>
+  <si>
+    <t>Should allow user to login</t>
+  </si>
+  <si>
+    <t>Should sent an email for recovering password</t>
+  </si>
+  <si>
+    <t>Verifying ‘Password reset’ functionality</t>
+  </si>
+  <si>
+    <t>Verifying change the password link is sent to valid email 
+address</t>
+  </si>
+  <si>
+    <t>Should be sent to valid email address</t>
+  </si>
+  <si>
+    <t>1. Go to https://dailyfinance.roadtocareer.net/
+2. Click on "reset it here" link</t>
+  </si>
+  <si>
+    <t>1. Go to https://dailyfinance.roadtocareer.net/
+2. Click on "reset it here" link
+3. Check the valid Email inbox</t>
+  </si>
+  <si>
+    <t>Verifying the functionality of 'Set a New Password'</t>
+  </si>
+  <si>
+    <t>Should provide a new input for setting new password</t>
+  </si>
+  <si>
+    <t>Verifying inputing old password on 'Set a New Password'</t>
+  </si>
+  <si>
+    <t>Should not allow user to login and display an error message</t>
+  </si>
+  <si>
+    <t>password got reset with old password</t>
+  </si>
+  <si>
+    <t>New password: "wizard0123"
+confirm password: "wizard0123"</t>
+  </si>
+  <si>
+    <t>New password: "wizard123"
+confirm password: "wizard123"</t>
+  </si>
+  <si>
+    <t>Verifying inputing new password on 'Set a New Password'</t>
+  </si>
+  <si>
+    <t>Should allow user to change the password</t>
+  </si>
+  <si>
+    <t>Verifying login with the newly changed password</t>
+  </si>
+  <si>
+    <t>Email: "testsofWizard@gmail.com"
+password: "wizard0123"</t>
+  </si>
+  <si>
+    <t>Checking if the link gets dissolved setting a new password</t>
+  </si>
+  <si>
+    <t>Link should get dissolved</t>
+  </si>
+  <si>
+    <t>Link is still active</t>
+  </si>
+  <si>
+    <t>1. Check the respective Email and click on the link again</t>
+  </si>
+  <si>
+    <t>TC61</t>
+  </si>
+  <si>
+    <t>TC62</t>
+  </si>
+  <si>
+    <t>TC63</t>
+  </si>
+  <si>
+    <t>TC64</t>
+  </si>
+  <si>
+    <t>TC65</t>
   </si>
 </sst>
 </file>
@@ -897,7 +1080,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -917,21 +1100,6 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -972,70 +1140,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1046,9 +1157,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1064,9 +1172,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1078,9 +1183,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1113,9 +1215,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1128,33 +1227,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1165,52 +1249,60 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1515,10 +1607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L58"/>
+  <dimension ref="A1:L79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,48 +1630,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="36" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="36" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="36" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="36" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="46"/>
+      <c r="B5" s="36"/>
     </row>
     <row r="6" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="46"/>
+      <c r="B6" s="36"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1624,31 +1716,31 @@
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" s="7" t="s">
+      <c r="H9" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="8" t="s">
         <v>58</v>
       </c>
       <c r="K9" s="2" t="s">
@@ -1660,25 +1752,25 @@
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="7" t="s">
+      <c r="B10" s="40"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I10" s="7" t="s">
+      <c r="H10" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J10" s="8" t="s">
         <v>58</v>
       </c>
       <c r="K10" s="2" t="s">
@@ -1690,25 +1782,25 @@
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="7" t="s">
+      <c r="B11" s="40"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H11" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I11" s="7" t="s">
+      <c r="H11" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="8" t="s">
         <v>58</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -1720,25 +1812,25 @@
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="57"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="7" t="s">
+      <c r="B12" s="40"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H12" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I12" s="7" t="s">
+      <c r="H12" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="9" t="s">
+      <c r="J12" s="8" t="s">
         <v>58</v>
       </c>
       <c r="K12" s="2" t="s">
@@ -1750,25 +1842,25 @@
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="7" t="s">
+      <c r="B13" s="40"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H13" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I13" s="7" t="s">
+      <c r="H13" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="J13" s="8" t="s">
         <v>58</v>
       </c>
       <c r="K13" s="2" t="s">
@@ -1780,25 +1872,25 @@
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="7" t="s">
+      <c r="B14" s="40"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H14" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" s="7" t="s">
+      <c r="H14" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="J14" s="6" t="s">
         <v>72</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -1810,25 +1902,25 @@
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="57"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="7" t="s">
+      <c r="B15" s="40"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H15" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15" s="7" t="s">
+      <c r="H15" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="J15" s="9" t="s">
+      <c r="J15" s="8" t="s">
         <v>58</v>
       </c>
       <c r="K15" s="2" t="s">
@@ -1840,25 +1932,25 @@
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="7" t="s">
+      <c r="B16" s="40"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H16" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="7" t="s">
+      <c r="H16" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J16" s="9" t="s">
+      <c r="J16" s="8" t="s">
         <v>58</v>
       </c>
       <c r="K16" s="2" t="s">
@@ -1870,25 +1962,25 @@
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="7" t="s">
+      <c r="B17" s="40"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H17" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I17" s="7" t="s">
+      <c r="H17" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J17" s="9" t="s">
+      <c r="J17" s="8" t="s">
         <v>58</v>
       </c>
       <c r="K17" s="2" t="s">
@@ -1900,25 +1992,25 @@
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="7" t="s">
+      <c r="B18" s="40"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H18" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I18" s="7" t="s">
+      <c r="H18" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I18" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="J18" s="7" t="s">
+      <c r="J18" s="6" t="s">
         <v>75</v>
       </c>
       <c r="K18" s="1" t="s">
@@ -1927,44 +2019,44 @@
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="5"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="4"/>
     </row>
     <row r="20" spans="1:12" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="57"/>
-      <c r="C20" s="55" t="s">
+      <c r="B20" s="40"/>
+      <c r="C20" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="54"/>
-      <c r="E20" s="7" t="s">
+      <c r="D20" s="37"/>
+      <c r="E20" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H20" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I20" s="7" t="s">
+      <c r="H20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J20" s="7" t="s">
+      <c r="J20" s="6" t="s">
         <v>58</v>
       </c>
       <c r="K20" s="1" t="s">
@@ -1976,25 +2068,25 @@
       <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="57"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="7" t="s">
+      <c r="B21" s="40"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H21" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I21" s="7" t="s">
+      <c r="H21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I21" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J21" s="7" t="s">
+      <c r="J21" s="6" t="s">
         <v>58</v>
       </c>
       <c r="K21" s="1" t="s">
@@ -2006,25 +2098,25 @@
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="58"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="7" t="s">
+      <c r="B22" s="41"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I22" s="7" t="s">
+      <c r="H22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="J22" s="6" t="s">
         <v>58</v>
       </c>
       <c r="K22" s="1" t="s">
@@ -2033,48 +2125,48 @@
       <c r="L22" s="2"/>
     </row>
     <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="12"/>
+      <c r="A23" s="46"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="10"/>
     </row>
     <row r="24" spans="1:12" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="59" t="s">
+      <c r="C24" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="50" t="s">
+      <c r="D24" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G24" s="11" t="s">
+      <c r="F24" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="H24" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I24" s="7" t="s">
+      <c r="H24" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="J24" s="9" t="s">
+      <c r="J24" s="8" t="s">
         <v>58</v>
       </c>
       <c r="K24" s="2" t="s">
@@ -2086,25 +2178,25 @@
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="51"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="7" t="s">
+      <c r="B25" s="47"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F25" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G25" s="7" t="s">
+      <c r="F25" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="H25" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I25" s="7" t="s">
+      <c r="H25" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I25" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J25" s="9" t="s">
+      <c r="J25" s="8" t="s">
         <v>58</v>
       </c>
       <c r="K25" s="2" t="s">
@@ -2116,25 +2208,25 @@
       <c r="A26" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="51"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="7" t="s">
+      <c r="B26" s="47"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G26" s="7" t="s">
+      <c r="F26" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="H26" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I26" s="7" t="s">
+      <c r="H26" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I26" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="J26" s="9" t="s">
+      <c r="J26" s="8" t="s">
         <v>58</v>
       </c>
       <c r="K26" s="2" t="s">
@@ -2146,922 +2238,1546 @@
       <c r="A27" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="51"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="7" t="s">
+      <c r="B27" s="47"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F27" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="G27" s="24" t="s">
+      <c r="F27" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="H27" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I27" s="7" t="s">
+      <c r="H27" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I27" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="J27" s="9" t="s">
+      <c r="J27" s="8" t="s">
         <v>58</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="L27" s="25"/>
+      <c r="L27" s="22"/>
     </row>
     <row r="28" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="51"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="10" t="s">
+      <c r="B28" s="47"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F28" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="G28" s="10" t="s">
+      <c r="F28" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="H28" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="I28" s="10" t="s">
+      <c r="H28" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I28" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="J28" s="10" t="s">
+      <c r="J28" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="K28" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="L28" s="15"/>
+      <c r="K28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="16" t="s">
+      <c r="B29" s="47"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F29" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G29" s="7" t="s">
+      <c r="F29" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G29" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="H29" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I29" s="7" t="s">
+      <c r="H29" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I29" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="J29" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="K29" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="L29" s="17"/>
+      <c r="J29" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K29" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L29" s="14"/>
     </row>
     <row r="30" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="51"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="16" t="s">
+      <c r="B30" s="47"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="F30" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G30" s="16" t="s">
+      <c r="F30" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G30" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H30" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I30" s="16" t="s">
+      <c r="H30" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I30" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="J30" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="K30" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="L30" s="17"/>
+      <c r="J30" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K30" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L30" s="14"/>
     </row>
     <row r="31" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="51"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="16" t="s">
+      <c r="B31" s="47"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="F31" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G31" s="16" t="s">
+      <c r="F31" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H31" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I31" s="16" t="s">
+      <c r="H31" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I31" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="J31" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="K31" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="L31" s="17"/>
+      <c r="J31" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K31" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L31" s="14"/>
     </row>
     <row r="32" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="51"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="19" t="s">
+      <c r="B32" s="47"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="F32" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G32" s="16" t="s">
+      <c r="F32" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G32" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H32" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I32" s="26" t="s">
+      <c r="H32" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I32" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="J32" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="K32" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="L32" s="17"/>
+      <c r="J32" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K32" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L32" s="14"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
-      <c r="B33" s="51"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
     </row>
     <row r="34" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="51"/>
-      <c r="C34" s="53" t="s">
+      <c r="B34" s="47"/>
+      <c r="C34" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="D34" s="51"/>
-      <c r="E34" s="29" t="s">
+      <c r="D34" s="48"/>
+      <c r="E34" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="F34" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G34" s="30" t="s">
+      <c r="F34" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G34" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="H34" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I34" s="18" t="s">
+      <c r="H34" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I34" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="J34" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="K34" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="L34" s="17"/>
+      <c r="J34" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K34" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L34" s="14"/>
     </row>
     <row r="35" spans="1:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="51"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="30" t="s">
+      <c r="B35" s="47"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="F35" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G35" s="30" t="s">
+      <c r="F35" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G35" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="H35" s="16" t="s">
+      <c r="H35" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="I35" s="18" t="s">
+      <c r="I35" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J35" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="K35" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="L35" s="17"/>
+      <c r="J35" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K35" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L35" s="14"/>
     </row>
     <row r="36" spans="1:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="51"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="30" t="s">
+      <c r="B36" s="47"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="F36" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G36" s="30" t="s">
+      <c r="F36" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G36" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="H36" s="16" t="s">
+      <c r="H36" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="I36" s="16" t="s">
+      <c r="I36" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="J36" s="16" t="s">
+      <c r="J36" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="K36" s="17" t="s">
+      <c r="K36" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="L36" s="17"/>
+      <c r="L36" s="14"/>
     </row>
     <row r="37" spans="1:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="51"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="30" t="s">
+      <c r="B37" s="47"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="F37" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G37" s="30" t="s">
+      <c r="F37" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G37" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="H37" s="16" t="s">
+      <c r="H37" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="I37" s="19" t="s">
+      <c r="I37" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="J37" s="16" t="s">
+      <c r="J37" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="K37" s="17" t="s">
+      <c r="K37" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="L37" s="17"/>
+      <c r="L37" s="14"/>
     </row>
     <row r="38" spans="1:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="51"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="30" t="s">
+      <c r="B38" s="47"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="F38" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G38" s="30" t="s">
+      <c r="F38" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G38" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="H38" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I38" s="16" t="s">
+      <c r="H38" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I38" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="J38" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="K38" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="L38" s="17"/>
+      <c r="J38" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K38" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L38" s="14"/>
     </row>
     <row r="39" spans="1:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="51"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="51"/>
-      <c r="E39" s="30" t="s">
+      <c r="B39" s="47"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="F39" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G39" s="30" t="s">
+      <c r="F39" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G39" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="H39" s="16" t="s">
+      <c r="H39" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="I39" s="16" t="s">
+      <c r="I39" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="J39" s="16" t="s">
+      <c r="J39" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="K39" s="17" t="s">
+      <c r="K39" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="L39" s="17"/>
+      <c r="L39" s="14"/>
     </row>
     <row r="40" spans="1:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="51"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="30" t="s">
+      <c r="B40" s="47"/>
+      <c r="C40" s="48"/>
+      <c r="D40" s="48"/>
+      <c r="E40" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="F40" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G40" s="30" t="s">
+      <c r="F40" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G40" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="H40" s="16" t="s">
+      <c r="H40" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="I40" s="16" t="s">
+      <c r="I40" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="J40" s="16" t="s">
+      <c r="J40" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="K40" s="17" t="s">
+      <c r="K40" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="L40" s="17"/>
+      <c r="L40" s="14"/>
     </row>
     <row r="41" spans="1:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="51"/>
-      <c r="C41" s="51"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="16" t="s">
+      <c r="B41" s="47"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="F41" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G41" s="30" t="s">
+      <c r="F41" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G41" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="H41" s="16" t="s">
+      <c r="H41" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="I41" s="18" t="s">
+      <c r="I41" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J41" s="18" t="s">
+      <c r="J41" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="K41" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="L41" s="17"/>
+      <c r="K41" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L41" s="14"/>
     </row>
     <row r="42" spans="1:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B42" s="51"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="30" t="s">
+      <c r="B42" s="47"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="F42" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G42" s="24" t="s">
+      <c r="F42" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G42" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="H42" s="16" t="s">
+      <c r="H42" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="I42" s="16" t="s">
+      <c r="I42" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="J42" s="16" t="s">
+      <c r="J42" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="K42" s="17" t="s">
+      <c r="K42" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="L42" s="25"/>
+      <c r="L42" s="22"/>
     </row>
     <row r="43" spans="1:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B43" s="51"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="51"/>
-      <c r="E43" s="30" t="s">
+      <c r="B43" s="47"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="F43" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G43" s="24" t="s">
+      <c r="F43" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G43" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="H43" s="16" t="s">
+      <c r="H43" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="I43" s="16" t="s">
+      <c r="I43" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="J43" s="16" t="s">
+      <c r="J43" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="K43" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="L43" s="25"/>
+      <c r="K43" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L43" s="22"/>
     </row>
     <row r="44" spans="1:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B44" s="51"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="51"/>
-      <c r="E44" s="30" t="s">
+      <c r="B44" s="47"/>
+      <c r="C44" s="48"/>
+      <c r="D44" s="48"/>
+      <c r="E44" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="F44" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G44" s="24" t="s">
+      <c r="F44" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G44" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="H44" s="16" t="s">
+      <c r="H44" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="I44" s="16" t="s">
+      <c r="I44" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="J44" s="16" t="s">
+      <c r="J44" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="K44" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="L44" s="25"/>
+      <c r="K44" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L44" s="22"/>
     </row>
     <row r="45" spans="1:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B45" s="51"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
-      <c r="E45" s="34" t="s">
+      <c r="B45" s="47"/>
+      <c r="C45" s="48"/>
+      <c r="D45" s="48"/>
+      <c r="E45" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="F45" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G45" s="24" t="s">
+      <c r="F45" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G45" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="H45" s="16" t="s">
+      <c r="H45" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="I45" s="18" t="s">
+      <c r="I45" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J45" s="18" t="s">
+      <c r="J45" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="K45" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="L45" s="25"/>
+      <c r="K45" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L45" s="22"/>
     </row>
     <row r="46" spans="1:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B46" s="51"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="34" t="s">
+      <c r="B46" s="47"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="F46" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G46" s="24" t="s">
+      <c r="F46" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G46" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="H46" s="16" t="s">
+      <c r="H46" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="I46" s="31" t="s">
+      <c r="I46" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J46" s="31" t="s">
+      <c r="J46" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="K46" s="35" t="s">
+      <c r="K46" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="L46" s="25"/>
+      <c r="L46" s="22"/>
     </row>
     <row r="47" spans="1:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B47" s="51"/>
-      <c r="C47" s="51"/>
-      <c r="D47" s="51"/>
-      <c r="E47" s="34" t="s">
+      <c r="B47" s="47"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="F47" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G47" s="24" t="s">
+      <c r="F47" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G47" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="H47" s="16" t="s">
+      <c r="H47" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="I47" s="18" t="s">
+      <c r="I47" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J47" s="16" t="s">
+      <c r="J47" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="K47" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="L47" s="25"/>
+      <c r="K47" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L47" s="22"/>
     </row>
     <row r="48" spans="1:12" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B48" s="51"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="51"/>
-      <c r="E48" s="31" t="s">
+      <c r="B48" s="47"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="F48" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G48" s="24" t="s">
+      <c r="F48" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G48" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="H48" s="16" t="s">
+      <c r="H48" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="I48" s="18" t="s">
+      <c r="I48" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J48" s="16" t="s">
+      <c r="J48" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="K48" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="L48" s="25"/>
+      <c r="K48" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L48" s="22"/>
     </row>
     <row r="49" spans="1:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B49" s="51"/>
-      <c r="C49" s="51"/>
-      <c r="D49" s="51"/>
-      <c r="E49" s="34" t="s">
+      <c r="B49" s="47"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="48"/>
+      <c r="E49" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="F49" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G49" s="24" t="s">
+      <c r="F49" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G49" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="H49" s="16" t="s">
+      <c r="H49" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="I49" s="16" t="s">
+      <c r="I49" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="J49" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="K49" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="L49" s="25"/>
+      <c r="J49" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K49" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L49" s="22"/>
     </row>
     <row r="50" spans="1:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B50" s="51"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="51"/>
-      <c r="E50" s="34" t="s">
+      <c r="B50" s="47"/>
+      <c r="C50" s="48"/>
+      <c r="D50" s="48"/>
+      <c r="E50" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="F50" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G50" s="24" t="s">
+      <c r="F50" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G50" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="H50" s="16" t="s">
+      <c r="H50" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="I50" s="16" t="s">
+      <c r="I50" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="J50" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="K50" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="L50" s="25"/>
+      <c r="J50" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K50" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L50" s="22"/>
     </row>
     <row r="51" spans="1:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B51" s="51"/>
-      <c r="C51" s="51"/>
-      <c r="D51" s="51"/>
-      <c r="E51" s="34" t="s">
+      <c r="B51" s="47"/>
+      <c r="C51" s="48"/>
+      <c r="D51" s="48"/>
+      <c r="E51" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="F51" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G51" s="24" t="s">
+      <c r="F51" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G51" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="H51" s="16" t="s">
+      <c r="H51" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="I51" s="31" t="s">
+      <c r="I51" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J51" s="31" t="s">
+      <c r="J51" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="K51" s="35" t="s">
+      <c r="K51" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="L51" s="25"/>
+      <c r="L51" s="22"/>
     </row>
     <row r="52" spans="1:12" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B52" s="51"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="32" t="s">
+      <c r="B52" s="47"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="48"/>
+      <c r="E52" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="F52" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G52" s="16" t="s">
+      <c r="F52" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G52" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="H52" s="16" t="s">
+      <c r="H52" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="I52" s="32" t="s">
+      <c r="I52" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="J52" s="31" t="s">
+      <c r="J52" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="K52" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="L52" s="25"/>
+      <c r="K52" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L52" s="22"/>
     </row>
     <row r="53" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B53" s="51"/>
-      <c r="C53" s="52"/>
-      <c r="D53" s="51"/>
-      <c r="E53" s="34" t="s">
+      <c r="B53" s="47"/>
+      <c r="C53" s="48"/>
+      <c r="D53" s="48"/>
+      <c r="E53" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="F53" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G53" s="24" t="s">
+      <c r="F53" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G53" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="H53" s="16" t="s">
+      <c r="H53" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="I53" s="32" t="s">
+      <c r="I53" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="J53" s="31" t="s">
+      <c r="J53" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="K53" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="L53" s="25"/>
+      <c r="K53" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L53" s="22"/>
     </row>
     <row r="54" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="5"/>
-      <c r="B54" s="51"/>
-      <c r="C54" s="40"/>
-      <c r="D54" s="51"/>
-      <c r="E54" s="41"/>
-      <c r="F54" s="21"/>
-      <c r="G54" s="42"/>
-      <c r="H54" s="42"/>
-      <c r="I54" s="43"/>
-      <c r="J54" s="21"/>
-      <c r="K54" s="22"/>
-      <c r="L54" s="44"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="47"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="48"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="33"/>
+      <c r="I54" s="34"/>
+      <c r="J54" s="18"/>
+      <c r="K54" s="19"/>
+      <c r="L54" s="35"/>
     </row>
     <row r="55" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B55" s="51"/>
-      <c r="C55" s="47" t="s">
+      <c r="B55" s="47"/>
+      <c r="C55" s="50" t="s">
         <v>162</v>
       </c>
-      <c r="D55" s="51"/>
-      <c r="E55" s="37" t="s">
+      <c r="D55" s="48"/>
+      <c r="E55" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="F55" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G55" s="16" t="s">
+      <c r="F55" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G55" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H55" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I55" s="38" t="s">
+      <c r="H55" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I55" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="J55" s="39" t="s">
+      <c r="J55" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="K55" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="L55" s="25"/>
+      <c r="K55" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L55" s="22"/>
     </row>
     <row r="56" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B56" s="51"/>
-      <c r="C56" s="48"/>
-      <c r="D56" s="51"/>
-      <c r="E56" s="36" t="s">
+      <c r="B56" s="47"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="48"/>
+      <c r="E56" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="F56" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G56" s="16" t="s">
+      <c r="F56" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G56" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H56" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I56" s="38" t="s">
+      <c r="H56" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I56" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="J56" s="39" t="s">
+      <c r="J56" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="K56" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="L56" s="25"/>
+      <c r="K56" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L56" s="22"/>
     </row>
     <row r="57" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B57" s="52"/>
-      <c r="C57" s="49"/>
-      <c r="D57" s="52"/>
-      <c r="E57" s="36" t="s">
+      <c r="B57" s="47"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="48"/>
+      <c r="E57" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="F57" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G57" s="16" t="s">
+      <c r="F57" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G57" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H57" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I57" s="38" t="s">
+      <c r="H57" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I57" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="J57" s="39" t="s">
+      <c r="J57" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="K57" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="L57" s="25"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="45"/>
-      <c r="C58" s="45"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="45"/>
-      <c r="F58" s="45"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="45"/>
-      <c r="I58" s="45"/>
-      <c r="J58" s="45"/>
-      <c r="K58" s="45"/>
-      <c r="L58" s="45"/>
+      <c r="K57" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="L57" s="22"/>
+    </row>
+    <row r="58" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="35"/>
+      <c r="B58" s="47"/>
+      <c r="C58" s="35"/>
+      <c r="D58" s="35"/>
+      <c r="E58" s="35"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="35"/>
+      <c r="H58" s="35"/>
+      <c r="I58" s="35"/>
+      <c r="J58" s="35"/>
+      <c r="K58" s="35"/>
+      <c r="L58" s="35"/>
+    </row>
+    <row r="59" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B59" s="47"/>
+      <c r="C59" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="D59" s="51" t="s">
+        <v>200</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H59" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I59" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J59" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L59" s="2"/>
+    </row>
+    <row r="60" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="B60" s="47"/>
+      <c r="C60" s="51"/>
+      <c r="D60" s="51"/>
+      <c r="E60" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H60" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J60" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L60" s="2"/>
+    </row>
+    <row r="61" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B61" s="47"/>
+      <c r="C61" s="51"/>
+      <c r="D61" s="51"/>
+      <c r="E61" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H61" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J61" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K61" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L61" s="2"/>
+    </row>
+    <row r="62" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B62" s="47"/>
+      <c r="C62" s="51"/>
+      <c r="D62" s="51"/>
+      <c r="E62" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F62" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="G62" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="H62" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I62" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J62" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L62" s="22"/>
+    </row>
+    <row r="63" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B63" s="47"/>
+      <c r="C63" s="51"/>
+      <c r="D63" s="51"/>
+      <c r="E63" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H63" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I63" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J63" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K63" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L63" s="2"/>
+    </row>
+    <row r="64" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B64" s="47"/>
+      <c r="C64" s="51"/>
+      <c r="D64" s="51"/>
+      <c r="E64" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H64" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I64" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="J64" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K64" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L64" s="14"/>
+    </row>
+    <row r="65" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B65" s="47"/>
+      <c r="C65" s="51"/>
+      <c r="D65" s="51"/>
+      <c r="E65" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F65" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="G65" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="H65" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I65" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="J65" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K65" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L65" s="14"/>
+    </row>
+    <row r="66" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="4"/>
+      <c r="B66" s="47"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="51"/>
+      <c r="E66" s="52"/>
+      <c r="F66" s="52"/>
+      <c r="G66" s="52"/>
+      <c r="H66" s="53"/>
+      <c r="I66" s="52"/>
+      <c r="J66" s="53"/>
+      <c r="K66" s="19"/>
+      <c r="L66" s="19"/>
+    </row>
+    <row r="67" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="B67" s="47"/>
+      <c r="C67" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="D67" s="51"/>
+      <c r="E67" s="43" t="s">
+        <v>202</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H67" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I67" s="43" t="s">
+        <v>203</v>
+      </c>
+      <c r="J67" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K67" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L67" s="22"/>
+    </row>
+    <row r="68" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B68" s="47"/>
+      <c r="C68" s="51"/>
+      <c r="D68" s="51"/>
+      <c r="E68" s="43" t="s">
+        <v>205</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H68" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="I68" s="43" t="s">
+        <v>203</v>
+      </c>
+      <c r="J68" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K68" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L68" s="22"/>
+    </row>
+    <row r="69" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="B69" s="47"/>
+      <c r="C69" s="51"/>
+      <c r="D69" s="51"/>
+      <c r="E69" s="43" t="s">
+        <v>207</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H69" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="I69" s="43" t="s">
+        <v>203</v>
+      </c>
+      <c r="J69" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K69" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L69" s="22"/>
+    </row>
+    <row r="70" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B70" s="47"/>
+      <c r="C70" s="51"/>
+      <c r="D70" s="51"/>
+      <c r="E70" s="44" t="s">
+        <v>204</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H70" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="I70" s="43" t="s">
+        <v>203</v>
+      </c>
+      <c r="J70" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K70" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L70" s="22"/>
+    </row>
+    <row r="71" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="B71" s="47"/>
+      <c r="C71" s="51"/>
+      <c r="D71" s="51"/>
+      <c r="E71" s="44" t="s">
+        <v>210</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H71" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="I71" s="43" t="s">
+        <v>212</v>
+      </c>
+      <c r="J71" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K71" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L71" s="22"/>
+    </row>
+    <row r="72" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B72" s="47"/>
+      <c r="C72" s="51"/>
+      <c r="D72" s="51"/>
+      <c r="E72" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H72" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="I72" s="43" t="s">
+        <v>215</v>
+      </c>
+      <c r="J72" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K72" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L72" s="22"/>
+    </row>
+    <row r="73" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="B73" s="47"/>
+      <c r="C73" s="51"/>
+      <c r="D73" s="51"/>
+      <c r="E73" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="H73" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I73" s="43" t="s">
+        <v>216</v>
+      </c>
+      <c r="J73" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="K73" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L73" s="22"/>
+    </row>
+    <row r="74" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B74" s="47"/>
+      <c r="C74" s="51"/>
+      <c r="D74" s="51"/>
+      <c r="E74" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="H74" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I74" s="43" t="s">
+        <v>219</v>
+      </c>
+      <c r="J74" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="K74" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L74" s="22"/>
+    </row>
+    <row r="75" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B75" s="47"/>
+      <c r="C75" s="51"/>
+      <c r="D75" s="51"/>
+      <c r="E75" s="44" t="s">
+        <v>222</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="H75" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I75" s="43" t="s">
+        <v>223</v>
+      </c>
+      <c r="J75" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="K75" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L75" s="22"/>
+    </row>
+    <row r="76" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B76" s="47"/>
+      <c r="C76" s="51"/>
+      <c r="D76" s="51"/>
+      <c r="E76" s="44" t="s">
+        <v>224</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="H76" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="I76" s="43" t="s">
+        <v>225</v>
+      </c>
+      <c r="J76" s="54" t="s">
+        <v>226</v>
+      </c>
+      <c r="K76" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L76" s="22"/>
+    </row>
+    <row r="77" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B77" s="47"/>
+      <c r="C77" s="51"/>
+      <c r="D77" s="51"/>
+      <c r="E77" s="44" t="s">
+        <v>229</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="H77" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="I77" s="54" t="s">
+        <v>230</v>
+      </c>
+      <c r="J77" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="K77" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L77" s="22"/>
+    </row>
+    <row r="78" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B78" s="47"/>
+      <c r="C78" s="51"/>
+      <c r="D78" s="51"/>
+      <c r="E78" s="43" t="s">
+        <v>231</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H78" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="I78" s="43" t="s">
+        <v>215</v>
+      </c>
+      <c r="J78" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="K78" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L78" s="22"/>
+    </row>
+    <row r="79" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B79" s="47"/>
+      <c r="C79" s="51"/>
+      <c r="D79" s="51"/>
+      <c r="E79" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="H79" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I79" s="43" t="s">
+        <v>234</v>
+      </c>
+      <c r="J79" s="54" t="s">
+        <v>235</v>
+      </c>
+      <c r="K79" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L79" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
+    <mergeCell ref="C59:C65"/>
+    <mergeCell ref="C67:C79"/>
+    <mergeCell ref="D59:D79"/>
+    <mergeCell ref="B24:B79"/>
     <mergeCell ref="C55:C57"/>
     <mergeCell ref="D24:D57"/>
-    <mergeCell ref="B24:B57"/>
     <mergeCell ref="C34:C53"/>
     <mergeCell ref="C9:C18"/>
     <mergeCell ref="D9:D22"/>

</xml_diff>

<commit_message>
dashboard module testcase added
</commit_message>
<xml_diff>
--- a/Test case report for Dailyfinance.net.xlsx
+++ b/Test case report for Dailyfinance.net.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="316">
   <si>
     <t>Project Name:</t>
   </si>
@@ -949,6 +949,267 @@
   </si>
   <si>
     <t>TC65</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Add Cost</t>
+  </si>
+  <si>
+    <t>1. Go to https://dailyfinance.roadtocareer.net/
+2. login with valid credentials
+3. click the "Add Cost" button</t>
+  </si>
+  <si>
+    <t>Not found as per expectation</t>
+  </si>
+  <si>
+    <t>Verifying mandatory field is marked with an asterisk sign</t>
+  </si>
+  <si>
+    <t>Not highlighted as per expectation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All input fields have lebel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All input fields have to associated with lebel </t>
+  </si>
+  <si>
+    <t>Do not behave responsive for smaller devices with viewport width below 560px</t>
+  </si>
+  <si>
+    <t>Keeping all input field blank</t>
+  </si>
+  <si>
+    <t>inputing numerical value in Item Name input</t>
+  </si>
+  <si>
+    <t>1. Homepage should be Active
+2. User have to be logged in</t>
+  </si>
+  <si>
+    <t>Item Name: "1"
+Quantity: "1"
+Amount: "100"
+Purchase Date: "10/25/2024"
+Month: "October"
+Remarks: " "</t>
+  </si>
+  <si>
+    <t>Should not let add a cost and
+display an error messeage</t>
+  </si>
+  <si>
+    <t>Item cost added</t>
+  </si>
+  <si>
+    <t>inputing alphabet in Item Name input</t>
+  </si>
+  <si>
+    <t>Item Name: "apple"
+Quantity: "1"
+Amount: "100"
+Purchase Date: "10/25/2024"
+Month: "October"
+Remarks: " "</t>
+  </si>
+  <si>
+    <t>Should let add a cost</t>
+  </si>
+  <si>
+    <t>Decremental button should be disable in quantity input</t>
+  </si>
+  <si>
+    <t>Decremental button should be disable in quantity input when quantity is 1</t>
+  </si>
+  <si>
+    <t>Decremental button should be enable in quantity input</t>
+  </si>
+  <si>
+    <t>Decremental button should be enable in quantity input when quantity is greater then 1</t>
+  </si>
+  <si>
+    <t>Should not let inputting any alphabet in amount field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inputing alphabet into amount input field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inputing numerical value in amount field </t>
+  </si>
+  <si>
+    <t>Amount field should take numerical value</t>
+  </si>
+  <si>
+    <t>amount field should not let put numerical negative value</t>
+  </si>
+  <si>
+    <t>Can put numerical negative value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numerical negative  value in amount field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">numerical "0" value in amount field </t>
+  </si>
+  <si>
+    <t>Item Name: "apple"
+Quantity: "1"
+Amount: "0"
+Purchase Date: "10/25/2024"
+Month: "October"
+Remarks: "This is for my brother "</t>
+  </si>
+  <si>
+    <t>Item Name: "apple"
+Quantity: "1"
+Amount: "20"
+Purchase Date: "10/25/2024"
+Month: "October"
+Remarks: "This is for my brother "</t>
+  </si>
+  <si>
+    <t>Inputing valid data for all mandatory inputs only</t>
+  </si>
+  <si>
+    <t>Item Name: "apple"
+Quantity: "1"
+Amount: "20"
+Purchase Date: "10/25/2024"
+Month: "October"</t>
+  </si>
+  <si>
+    <t>Keeping amount input field blank</t>
+  </si>
+  <si>
+    <t>Item Name: "apple"
+Quantity: "1"
+Amount: " "
+Purchase Date: "10/25/2024"
+Month: "October"
+Remarks: "This is for my brother"</t>
+  </si>
+  <si>
+    <t>Date picker in Purchase Date field should let change date</t>
+  </si>
+  <si>
+    <t>Date picker functionality in Purchase Date field</t>
+  </si>
+  <si>
+    <t>Date picker in Purchase Date field should let clear out date</t>
+  </si>
+  <si>
+    <t>Date picker should format the date in "MM/DD/YYYY"</t>
+  </si>
+  <si>
+    <t>Month field functionality</t>
+  </si>
+  <si>
+    <t>Month field should let change the month</t>
+  </si>
+  <si>
+    <t>date picker Should have today's value by default</t>
+  </si>
+  <si>
+    <t>Should let add a cost and
+display an error messeage</t>
+  </si>
+  <si>
+    <t>date picker Should have current month value by default</t>
+  </si>
+  <si>
+    <t>Reset button resets input value</t>
+  </si>
+  <si>
+    <t>Item Name: "apple"
+Quantity: "2"
+Amount: "50"
+Purchase Date: "10/25/2024"
+Month: "October"
+Remarks: "This is for my brother "</t>
+  </si>
+  <si>
+    <t>Reset button should reset all input value except those who have default value</t>
+  </si>
+  <si>
+    <t>TC66</t>
+  </si>
+  <si>
+    <t>TC67</t>
+  </si>
+  <si>
+    <t>TC68</t>
+  </si>
+  <si>
+    <t>TC69</t>
+  </si>
+  <si>
+    <t>TC70</t>
+  </si>
+  <si>
+    <t>TC71</t>
+  </si>
+  <si>
+    <t>TC72</t>
+  </si>
+  <si>
+    <t>TC73</t>
+  </si>
+  <si>
+    <t>TC74</t>
+  </si>
+  <si>
+    <t>TC75</t>
+  </si>
+  <si>
+    <t>TC76</t>
+  </si>
+  <si>
+    <t>TC77</t>
+  </si>
+  <si>
+    <t>TC78</t>
+  </si>
+  <si>
+    <t>TC79</t>
+  </si>
+  <si>
+    <t>TC80</t>
+  </si>
+  <si>
+    <t>TC81</t>
+  </si>
+  <si>
+    <t>TC82</t>
+  </si>
+  <si>
+    <t>TC83</t>
+  </si>
+  <si>
+    <t>TC84</t>
+  </si>
+  <si>
+    <t>TC85</t>
+  </si>
+  <si>
+    <t>TC86</t>
+  </si>
+  <si>
+    <t>TC87</t>
+  </si>
+  <si>
+    <t>TC88</t>
+  </si>
+  <si>
+    <t>TC89</t>
+  </si>
+  <si>
+    <t>TC90</t>
+  </si>
+  <si>
+    <t>TC91</t>
   </si>
 </sst>
 </file>
@@ -1146,7 +1407,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1250,6 +1511,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1265,44 +1565,12 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1607,10 +1875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L79"/>
+  <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O105" sqref="O105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1716,13 +1984,13 @@
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="50" t="s">
         <v>53</v>
       </c>
       <c r="E9" s="6" t="s">
@@ -1752,9 +2020,9 @@
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
       <c r="E10" s="6" t="s">
         <v>60</v>
       </c>
@@ -1782,9 +2050,9 @@
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
       <c r="E11" s="6" t="s">
         <v>62</v>
       </c>
@@ -1812,9 +2080,9 @@
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
       <c r="E12" s="6" t="s">
         <v>63</v>
       </c>
@@ -1842,9 +2110,9 @@
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
       <c r="E13" s="6" t="s">
         <v>64</v>
       </c>
@@ -1872,9 +2140,9 @@
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
       <c r="E14" s="6" t="s">
         <v>65</v>
       </c>
@@ -1902,9 +2170,9 @@
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
       <c r="E15" s="6" t="s">
         <v>66</v>
       </c>
@@ -1932,9 +2200,9 @@
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
       <c r="E16" s="6" t="s">
         <v>67</v>
       </c>
@@ -1962,9 +2230,9 @@
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
       <c r="E17" s="6" t="s">
         <v>68</v>
       </c>
@@ -1992,9 +2260,9 @@
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
       <c r="E18" s="6" t="s">
         <v>73</v>
       </c>
@@ -2020,9 +2288,9 @@
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
-      <c r="B19" s="40"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="37"/>
+      <c r="D19" s="50"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
@@ -2036,11 +2304,11 @@
       <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="38" t="s">
+      <c r="B20" s="53"/>
+      <c r="C20" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="37"/>
+      <c r="D20" s="50"/>
       <c r="E20" s="6" t="s">
         <v>78</v>
       </c>
@@ -2068,9 +2336,9 @@
       <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="37"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="50"/>
       <c r="E21" s="6" t="s">
         <v>79</v>
       </c>
@@ -2098,9 +2366,9 @@
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="37"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="50"/>
       <c r="E22" s="6" t="s">
         <v>80</v>
       </c>
@@ -2125,7 +2393,7 @@
       <c r="L22" s="2"/>
     </row>
     <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="46"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
       <c r="D23" s="10"/>
@@ -2145,10 +2413,10 @@
       <c r="B24" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="48" t="s">
+      <c r="C24" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="48" t="s">
+      <c r="D24" s="49" t="s">
         <v>82</v>
       </c>
       <c r="E24" s="6" t="s">
@@ -2179,8 +2447,8 @@
         <v>35</v>
       </c>
       <c r="B25" s="47"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
       <c r="E25" s="6" t="s">
         <v>60</v>
       </c>
@@ -2209,8 +2477,8 @@
         <v>36</v>
       </c>
       <c r="B26" s="47"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
       <c r="E26" s="6" t="s">
         <v>64</v>
       </c>
@@ -2239,8 +2507,8 @@
         <v>37</v>
       </c>
       <c r="B27" s="47"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
       <c r="E27" s="6" t="s">
         <v>66</v>
       </c>
@@ -2269,8 +2537,8 @@
         <v>38</v>
       </c>
       <c r="B28" s="47"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
       <c r="E28" s="6" t="s">
         <v>65</v>
       </c>
@@ -2299,8 +2567,8 @@
         <v>39</v>
       </c>
       <c r="B29" s="47"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
       <c r="E29" s="13" t="s">
         <v>87</v>
       </c>
@@ -2329,8 +2597,8 @@
         <v>40</v>
       </c>
       <c r="B30" s="47"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
       <c r="E30" s="13" t="s">
         <v>73</v>
       </c>
@@ -2359,8 +2627,8 @@
         <v>41</v>
       </c>
       <c r="B31" s="47"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
       <c r="E31" s="13" t="s">
         <v>90</v>
       </c>
@@ -2389,8 +2657,8 @@
         <v>42</v>
       </c>
       <c r="B32" s="47"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
       <c r="E32" s="16" t="s">
         <v>89</v>
       </c>
@@ -2418,7 +2686,7 @@
       <c r="A33" s="4"/>
       <c r="B33" s="47"/>
       <c r="C33" s="19"/>
-      <c r="D33" s="48"/>
+      <c r="D33" s="49"/>
       <c r="E33" s="17"/>
       <c r="F33" s="18"/>
       <c r="G33" s="18"/>
@@ -2433,10 +2701,10 @@
         <v>43</v>
       </c>
       <c r="B34" s="47"/>
-      <c r="C34" s="48" t="s">
+      <c r="C34" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="D34" s="48"/>
+      <c r="D34" s="49"/>
       <c r="E34" s="25" t="s">
         <v>95</v>
       </c>
@@ -2465,8 +2733,8 @@
         <v>44</v>
       </c>
       <c r="B35" s="47"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
       <c r="E35" s="26" t="s">
         <v>96</v>
       </c>
@@ -2495,8 +2763,8 @@
         <v>45</v>
       </c>
       <c r="B36" s="47"/>
-      <c r="C36" s="48"/>
-      <c r="D36" s="48"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
       <c r="E36" s="26" t="s">
         <v>99</v>
       </c>
@@ -2525,8 +2793,8 @@
         <v>46</v>
       </c>
       <c r="B37" s="47"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
       <c r="E37" s="26" t="s">
         <v>103</v>
       </c>
@@ -2555,8 +2823,8 @@
         <v>47</v>
       </c>
       <c r="B38" s="47"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="48"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
       <c r="E38" s="26" t="s">
         <v>105</v>
       </c>
@@ -2585,8 +2853,8 @@
         <v>48</v>
       </c>
       <c r="B39" s="47"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
       <c r="E39" s="26" t="s">
         <v>108</v>
       </c>
@@ -2615,8 +2883,8 @@
         <v>49</v>
       </c>
       <c r="B40" s="47"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="48"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
       <c r="E40" s="26" t="s">
         <v>113</v>
       </c>
@@ -2645,8 +2913,8 @@
         <v>50</v>
       </c>
       <c r="B41" s="47"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
       <c r="E41" s="13" t="s">
         <v>116</v>
       </c>
@@ -2675,8 +2943,8 @@
         <v>119</v>
       </c>
       <c r="B42" s="47"/>
-      <c r="C42" s="48"/>
-      <c r="D42" s="48"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="49"/>
       <c r="E42" s="26" t="s">
         <v>118</v>
       </c>
@@ -2705,8 +2973,8 @@
         <v>120</v>
       </c>
       <c r="B43" s="47"/>
-      <c r="C43" s="48"/>
-      <c r="D43" s="48"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="49"/>
       <c r="E43" s="26" t="s">
         <v>123</v>
       </c>
@@ -2735,8 +3003,8 @@
         <v>127</v>
       </c>
       <c r="B44" s="47"/>
-      <c r="C44" s="48"/>
-      <c r="D44" s="48"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="49"/>
       <c r="E44" s="26" t="s">
         <v>131</v>
       </c>
@@ -2765,8 +3033,8 @@
         <v>128</v>
       </c>
       <c r="B45" s="47"/>
-      <c r="C45" s="48"/>
-      <c r="D45" s="48"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="49"/>
       <c r="E45" s="28" t="s">
         <v>133</v>
       </c>
@@ -2795,8 +3063,8 @@
         <v>129</v>
       </c>
       <c r="B46" s="47"/>
-      <c r="C46" s="48"/>
-      <c r="D46" s="48"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="49"/>
       <c r="E46" s="28" t="s">
         <v>136</v>
       </c>
@@ -2825,8 +3093,8 @@
         <v>130</v>
       </c>
       <c r="B47" s="47"/>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="49"/>
       <c r="E47" s="28" t="s">
         <v>137</v>
       </c>
@@ -2855,8 +3123,8 @@
         <v>149</v>
       </c>
       <c r="B48" s="47"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="49"/>
       <c r="E48" s="27" t="s">
         <v>138</v>
       </c>
@@ -2885,8 +3153,8 @@
         <v>150</v>
       </c>
       <c r="B49" s="47"/>
-      <c r="C49" s="48"/>
-      <c r="D49" s="48"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="49"/>
       <c r="E49" s="28" t="s">
         <v>140</v>
       </c>
@@ -2915,8 +3183,8 @@
         <v>151</v>
       </c>
       <c r="B50" s="47"/>
-      <c r="C50" s="48"/>
-      <c r="D50" s="48"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="49"/>
       <c r="E50" s="28" t="s">
         <v>144</v>
       </c>
@@ -2945,8 +3213,8 @@
         <v>152</v>
       </c>
       <c r="B51" s="47"/>
-      <c r="C51" s="48"/>
-      <c r="D51" s="48"/>
+      <c r="C51" s="49"/>
+      <c r="D51" s="49"/>
       <c r="E51" s="28" t="s">
         <v>146</v>
       </c>
@@ -2975,8 +3243,8 @@
         <v>160</v>
       </c>
       <c r="B52" s="47"/>
-      <c r="C52" s="48"/>
-      <c r="D52" s="48"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="49"/>
       <c r="E52" s="30" t="s">
         <v>153</v>
       </c>
@@ -3005,8 +3273,8 @@
         <v>161</v>
       </c>
       <c r="B53" s="47"/>
-      <c r="C53" s="48"/>
-      <c r="D53" s="48"/>
+      <c r="C53" s="49"/>
+      <c r="D53" s="49"/>
       <c r="E53" s="28" t="s">
         <v>157</v>
       </c>
@@ -3033,8 +3301,8 @@
     <row r="54" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
       <c r="B54" s="47"/>
-      <c r="C54" s="49"/>
-      <c r="D54" s="48"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="49"/>
       <c r="E54" s="32"/>
       <c r="F54" s="18"/>
       <c r="G54" s="33"/>
@@ -3049,10 +3317,10 @@
         <v>170</v>
       </c>
       <c r="B55" s="47"/>
-      <c r="C55" s="50" t="s">
+      <c r="C55" s="48" t="s">
         <v>162</v>
       </c>
-      <c r="D55" s="48"/>
+      <c r="D55" s="49"/>
       <c r="E55" s="31" t="s">
         <v>163</v>
       </c>
@@ -3081,8 +3349,8 @@
         <v>171</v>
       </c>
       <c r="B56" s="47"/>
-      <c r="C56" s="50"/>
-      <c r="D56" s="48"/>
+      <c r="C56" s="48"/>
+      <c r="D56" s="49"/>
       <c r="E56" s="30" t="s">
         <v>164</v>
       </c>
@@ -3111,8 +3379,8 @@
         <v>172</v>
       </c>
       <c r="B57" s="47"/>
-      <c r="C57" s="50"/>
-      <c r="D57" s="48"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="49"/>
       <c r="E57" s="30" t="s">
         <v>165</v>
       </c>
@@ -3155,10 +3423,10 @@
         <v>185</v>
       </c>
       <c r="B59" s="47"/>
-      <c r="C59" s="51" t="s">
+      <c r="C59" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="D59" s="51" t="s">
+      <c r="D59" s="49" t="s">
         <v>200</v>
       </c>
       <c r="E59" s="6" t="s">
@@ -3189,8 +3457,8 @@
         <v>186</v>
       </c>
       <c r="B60" s="47"/>
-      <c r="C60" s="51"/>
-      <c r="D60" s="51"/>
+      <c r="C60" s="49"/>
+      <c r="D60" s="49"/>
       <c r="E60" s="6" t="s">
         <v>60</v>
       </c>
@@ -3219,10 +3487,10 @@
         <v>187</v>
       </c>
       <c r="B61" s="47"/>
-      <c r="C61" s="51"/>
-      <c r="D61" s="51"/>
+      <c r="C61" s="49"/>
+      <c r="D61" s="49"/>
       <c r="E61" s="6" t="s">
-        <v>64</v>
+        <v>246</v>
       </c>
       <c r="F61" s="9" t="s">
         <v>88</v>
@@ -3249,12 +3517,12 @@
         <v>188</v>
       </c>
       <c r="B62" s="47"/>
-      <c r="C62" s="51"/>
-      <c r="D62" s="51"/>
+      <c r="C62" s="49"/>
+      <c r="D62" s="49"/>
       <c r="E62" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F62" s="42" t="s">
+      <c r="F62" s="37" t="s">
         <v>88</v>
       </c>
       <c r="G62" s="13" t="s">
@@ -3279,8 +3547,8 @@
         <v>189</v>
       </c>
       <c r="B63" s="47"/>
-      <c r="C63" s="51"/>
-      <c r="D63" s="51"/>
+      <c r="C63" s="49"/>
+      <c r="D63" s="49"/>
       <c r="E63" s="6" t="s">
         <v>65</v>
       </c>
@@ -3309,8 +3577,8 @@
         <v>190</v>
       </c>
       <c r="B64" s="47"/>
-      <c r="C64" s="51"/>
-      <c r="D64" s="51"/>
+      <c r="C64" s="49"/>
+      <c r="D64" s="49"/>
       <c r="E64" s="13" t="s">
         <v>87</v>
       </c>
@@ -3339,12 +3607,12 @@
         <v>191</v>
       </c>
       <c r="B65" s="47"/>
-      <c r="C65" s="51"/>
-      <c r="D65" s="51"/>
+      <c r="C65" s="49"/>
+      <c r="D65" s="49"/>
       <c r="E65" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="F65" s="42" t="s">
+      <c r="F65" s="37" t="s">
         <v>88</v>
       </c>
       <c r="G65" s="13" t="s">
@@ -3368,13 +3636,13 @@
       <c r="A66" s="4"/>
       <c r="B66" s="47"/>
       <c r="C66" s="19"/>
-      <c r="D66" s="51"/>
-      <c r="E66" s="52"/>
-      <c r="F66" s="52"/>
-      <c r="G66" s="52"/>
-      <c r="H66" s="53"/>
-      <c r="I66" s="52"/>
-      <c r="J66" s="53"/>
+      <c r="D66" s="49"/>
+      <c r="E66" s="44"/>
+      <c r="F66" s="44"/>
+      <c r="G66" s="44"/>
+      <c r="H66" s="45"/>
+      <c r="I66" s="44"/>
+      <c r="J66" s="45"/>
       <c r="K66" s="19"/>
       <c r="L66" s="19"/>
     </row>
@@ -3383,11 +3651,11 @@
         <v>192</v>
       </c>
       <c r="B67" s="47"/>
-      <c r="C67" s="51" t="s">
+      <c r="C67" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="D67" s="51"/>
-      <c r="E67" s="43" t="s">
+      <c r="D67" s="49"/>
+      <c r="E67" s="38" t="s">
         <v>202</v>
       </c>
       <c r="F67" s="6" t="s">
@@ -3399,7 +3667,7 @@
       <c r="H67" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="I67" s="43" t="s">
+      <c r="I67" s="38" t="s">
         <v>203</v>
       </c>
       <c r="J67" s="15" t="s">
@@ -3415,9 +3683,9 @@
         <v>193</v>
       </c>
       <c r="B68" s="47"/>
-      <c r="C68" s="51"/>
-      <c r="D68" s="51"/>
-      <c r="E68" s="43" t="s">
+      <c r="C68" s="49"/>
+      <c r="D68" s="49"/>
+      <c r="E68" s="38" t="s">
         <v>205</v>
       </c>
       <c r="F68" s="6" t="s">
@@ -3429,7 +3697,7 @@
       <c r="H68" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="I68" s="43" t="s">
+      <c r="I68" s="38" t="s">
         <v>203</v>
       </c>
       <c r="J68" s="15" t="s">
@@ -3440,14 +3708,14 @@
       </c>
       <c r="L68" s="22"/>
     </row>
-    <row r="69" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="14" t="s">
         <v>194</v>
       </c>
       <c r="B69" s="47"/>
-      <c r="C69" s="51"/>
-      <c r="D69" s="51"/>
-      <c r="E69" s="43" t="s">
+      <c r="C69" s="49"/>
+      <c r="D69" s="49"/>
+      <c r="E69" s="38" t="s">
         <v>207</v>
       </c>
       <c r="F69" s="6" t="s">
@@ -3459,7 +3727,7 @@
       <c r="H69" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="I69" s="43" t="s">
+      <c r="I69" s="38" t="s">
         <v>203</v>
       </c>
       <c r="J69" s="15" t="s">
@@ -3475,9 +3743,9 @@
         <v>195</v>
       </c>
       <c r="B70" s="47"/>
-      <c r="C70" s="51"/>
-      <c r="D70" s="51"/>
-      <c r="E70" s="44" t="s">
+      <c r="C70" s="49"/>
+      <c r="D70" s="49"/>
+      <c r="E70" s="39" t="s">
         <v>204</v>
       </c>
       <c r="F70" s="6" t="s">
@@ -3489,7 +3757,7 @@
       <c r="H70" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="I70" s="43" t="s">
+      <c r="I70" s="38" t="s">
         <v>203</v>
       </c>
       <c r="J70" s="15" t="s">
@@ -3505,9 +3773,9 @@
         <v>196</v>
       </c>
       <c r="B71" s="47"/>
-      <c r="C71" s="51"/>
-      <c r="D71" s="51"/>
-      <c r="E71" s="44" t="s">
+      <c r="C71" s="49"/>
+      <c r="D71" s="49"/>
+      <c r="E71" s="39" t="s">
         <v>210</v>
       </c>
       <c r="F71" s="6" t="s">
@@ -3519,7 +3787,7 @@
       <c r="H71" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="I71" s="43" t="s">
+      <c r="I71" s="38" t="s">
         <v>212</v>
       </c>
       <c r="J71" s="15" t="s">
@@ -3535,9 +3803,9 @@
         <v>197</v>
       </c>
       <c r="B72" s="47"/>
-      <c r="C72" s="51"/>
-      <c r="D72" s="51"/>
-      <c r="E72" s="44" t="s">
+      <c r="C72" s="49"/>
+      <c r="D72" s="49"/>
+      <c r="E72" s="39" t="s">
         <v>213</v>
       </c>
       <c r="F72" s="6" t="s">
@@ -3549,7 +3817,7 @@
       <c r="H72" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="I72" s="43" t="s">
+      <c r="I72" s="38" t="s">
         <v>215</v>
       </c>
       <c r="J72" s="15" t="s">
@@ -3565,9 +3833,9 @@
         <v>198</v>
       </c>
       <c r="B73" s="47"/>
-      <c r="C73" s="51"/>
-      <c r="D73" s="51"/>
-      <c r="E73" s="44" t="s">
+      <c r="C73" s="49"/>
+      <c r="D73" s="49"/>
+      <c r="E73" s="39" t="s">
         <v>217</v>
       </c>
       <c r="F73" s="6" t="s">
@@ -3579,10 +3847,10 @@
       <c r="H73" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="I73" s="43" t="s">
+      <c r="I73" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="J73" s="43" t="s">
+      <c r="J73" s="38" t="s">
         <v>58</v>
       </c>
       <c r="K73" s="14" t="s">
@@ -3595,9 +3863,9 @@
         <v>199</v>
       </c>
       <c r="B74" s="47"/>
-      <c r="C74" s="51"/>
-      <c r="D74" s="51"/>
-      <c r="E74" s="44" t="s">
+      <c r="C74" s="49"/>
+      <c r="D74" s="49"/>
+      <c r="E74" s="39" t="s">
         <v>218</v>
       </c>
       <c r="F74" s="6" t="s">
@@ -3609,10 +3877,10 @@
       <c r="H74" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="I74" s="43" t="s">
+      <c r="I74" s="38" t="s">
         <v>219</v>
       </c>
-      <c r="J74" s="45" t="s">
+      <c r="J74" s="40" t="s">
         <v>58</v>
       </c>
       <c r="K74" s="14" t="s">
@@ -3625,9 +3893,9 @@
         <v>237</v>
       </c>
       <c r="B75" s="47"/>
-      <c r="C75" s="51"/>
-      <c r="D75" s="51"/>
-      <c r="E75" s="44" t="s">
+      <c r="C75" s="49"/>
+      <c r="D75" s="49"/>
+      <c r="E75" s="39" t="s">
         <v>222</v>
       </c>
       <c r="F75" s="6" t="s">
@@ -3639,10 +3907,10 @@
       <c r="H75" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="I75" s="43" t="s">
+      <c r="I75" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="J75" s="43" t="s">
+      <c r="J75" s="38" t="s">
         <v>58</v>
       </c>
       <c r="K75" s="14" t="s">
@@ -3655,9 +3923,9 @@
         <v>238</v>
       </c>
       <c r="B76" s="47"/>
-      <c r="C76" s="51"/>
-      <c r="D76" s="51"/>
-      <c r="E76" s="44" t="s">
+      <c r="C76" s="49"/>
+      <c r="D76" s="49"/>
+      <c r="E76" s="39" t="s">
         <v>224</v>
       </c>
       <c r="F76" s="6" t="s">
@@ -3669,10 +3937,10 @@
       <c r="H76" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="I76" s="43" t="s">
+      <c r="I76" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="J76" s="54" t="s">
+      <c r="J76" s="46" t="s">
         <v>226</v>
       </c>
       <c r="K76" s="14" t="s">
@@ -3685,9 +3953,9 @@
         <v>239</v>
       </c>
       <c r="B77" s="47"/>
-      <c r="C77" s="51"/>
-      <c r="D77" s="51"/>
-      <c r="E77" s="44" t="s">
+      <c r="C77" s="49"/>
+      <c r="D77" s="49"/>
+      <c r="E77" s="39" t="s">
         <v>229</v>
       </c>
       <c r="F77" s="6" t="s">
@@ -3699,10 +3967,10 @@
       <c r="H77" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="I77" s="54" t="s">
+      <c r="I77" s="46" t="s">
         <v>230</v>
       </c>
-      <c r="J77" s="43" t="s">
+      <c r="J77" s="38" t="s">
         <v>58</v>
       </c>
       <c r="K77" s="14" t="s">
@@ -3715,9 +3983,9 @@
         <v>240</v>
       </c>
       <c r="B78" s="47"/>
-      <c r="C78" s="51"/>
-      <c r="D78" s="51"/>
-      <c r="E78" s="43" t="s">
+      <c r="C78" s="49"/>
+      <c r="D78" s="49"/>
+      <c r="E78" s="38" t="s">
         <v>231</v>
       </c>
       <c r="F78" s="6" t="s">
@@ -3729,10 +3997,10 @@
       <c r="H78" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="I78" s="43" t="s">
+      <c r="I78" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="J78" s="43" t="s">
+      <c r="J78" s="38" t="s">
         <v>58</v>
       </c>
       <c r="K78" s="14" t="s">
@@ -3745,9 +4013,9 @@
         <v>241</v>
       </c>
       <c r="B79" s="47"/>
-      <c r="C79" s="51"/>
-      <c r="D79" s="51"/>
-      <c r="E79" s="44" t="s">
+      <c r="C79" s="49"/>
+      <c r="D79" s="49"/>
+      <c r="E79" s="39" t="s">
         <v>233</v>
       </c>
       <c r="F79" s="6" t="s">
@@ -3759,10 +4027,10 @@
       <c r="H79" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="I79" s="43" t="s">
+      <c r="I79" s="38" t="s">
         <v>234</v>
       </c>
-      <c r="J79" s="54" t="s">
+      <c r="J79" s="46" t="s">
         <v>235</v>
       </c>
       <c r="K79" s="14" t="s">
@@ -3770,8 +4038,863 @@
       </c>
       <c r="L79" s="22"/>
     </row>
+    <row r="80" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="55"/>
+      <c r="C80" s="55"/>
+      <c r="D80" s="55"/>
+      <c r="E80" s="55"/>
+      <c r="F80" s="55"/>
+      <c r="G80" s="55"/>
+      <c r="H80" s="55"/>
+      <c r="I80" s="55"/>
+      <c r="J80" s="55"/>
+      <c r="K80" s="55"/>
+      <c r="L80" s="55"/>
+    </row>
+    <row r="81" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B81" s="49" t="s">
+        <v>242</v>
+      </c>
+      <c r="C81" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="D81" s="49" t="s">
+        <v>243</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H81" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I81" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J81" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K81" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L81" s="22"/>
+    </row>
+    <row r="82" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B82" s="49"/>
+      <c r="C82" s="49"/>
+      <c r="D82" s="49"/>
+      <c r="E82" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H82" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I82" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J82" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K82" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L82" s="22"/>
+    </row>
+    <row r="83" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B83" s="49"/>
+      <c r="C83" s="49"/>
+      <c r="D83" s="49"/>
+      <c r="E83" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H83" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I83" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J83" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="K83" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L83" s="22"/>
+    </row>
+    <row r="84" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B84" s="49"/>
+      <c r="C84" s="49"/>
+      <c r="D84" s="49"/>
+      <c r="E84" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G84" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H84" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I84" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J84" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K84" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L84" s="22"/>
+    </row>
+    <row r="85" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B85" s="49"/>
+      <c r="C85" s="49"/>
+      <c r="D85" s="49"/>
+      <c r="E85" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G85" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H85" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I85" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J85" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="K85" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L85" s="22"/>
+    </row>
+    <row r="86" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B86" s="49"/>
+      <c r="C86" s="49"/>
+      <c r="D86" s="49"/>
+      <c r="E86" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H86" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I86" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="J86" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K86" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="L86" s="22"/>
+    </row>
+    <row r="87" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B87" s="49"/>
+      <c r="C87" s="49"/>
+      <c r="D87" s="49"/>
+      <c r="E87" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G87" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H87" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I87" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="J87" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="K87" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L87" s="22"/>
+    </row>
+    <row r="88" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="22"/>
+      <c r="B88" s="49"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="49"/>
+      <c r="E88" s="24"/>
+      <c r="F88" s="24"/>
+      <c r="G88" s="24"/>
+      <c r="H88" s="24"/>
+      <c r="I88" s="24"/>
+      <c r="J88" s="24"/>
+      <c r="K88" s="19"/>
+      <c r="L88" s="35"/>
+    </row>
+    <row r="89" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B89" s="49"/>
+      <c r="C89" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="D89" s="49"/>
+      <c r="E89" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G89" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H89" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I89" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="J89" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K89" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="L89" s="22"/>
+    </row>
+    <row r="90" spans="1:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B90" s="49"/>
+      <c r="C90" s="49"/>
+      <c r="D90" s="49"/>
+      <c r="E90" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="F90" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G90" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H90" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="I90" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="J90" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L90" s="22"/>
+    </row>
+    <row r="91" spans="1:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B91" s="49"/>
+      <c r="C91" s="49"/>
+      <c r="D91" s="49"/>
+      <c r="E91" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="F91" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G91" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H91" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="I91" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="J91" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K91" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="L91" s="22"/>
+    </row>
+    <row r="92" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B92" s="49"/>
+      <c r="C92" s="49"/>
+      <c r="D92" s="49"/>
+      <c r="E92" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G92" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H92" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I92" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="J92" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K92" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="L92" s="22"/>
+    </row>
+    <row r="93" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B93" s="49"/>
+      <c r="C93" s="49"/>
+      <c r="D93" s="49"/>
+      <c r="E93" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G93" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H93" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I93" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="J93" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K93" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="L93" s="22"/>
+    </row>
+    <row r="94" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B94" s="49"/>
+      <c r="C94" s="49"/>
+      <c r="D94" s="49"/>
+      <c r="E94" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="F94" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G94" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H94" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I94" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="J94" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K94" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="L94" s="22"/>
+    </row>
+    <row r="95" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B95" s="49"/>
+      <c r="C95" s="49"/>
+      <c r="D95" s="49"/>
+      <c r="E95" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="F95" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G95" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H95" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I95" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="J95" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K95" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="L95" s="22"/>
+    </row>
+    <row r="96" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B96" s="49"/>
+      <c r="C96" s="49"/>
+      <c r="D96" s="49"/>
+      <c r="E96" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="F96" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G96" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H96" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I96" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="J96" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="K96" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L96" s="22"/>
+    </row>
+    <row r="97" spans="1:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B97" s="49"/>
+      <c r="C97" s="49"/>
+      <c r="D97" s="49"/>
+      <c r="E97" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="F97" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G97" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H97" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="I97" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="J97" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="K97" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L97" s="22"/>
+    </row>
+    <row r="98" spans="1:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B98" s="49"/>
+      <c r="C98" s="49"/>
+      <c r="D98" s="49"/>
+      <c r="E98" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="F98" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G98" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H98" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="I98" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="J98" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K98" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="L98" s="22"/>
+    </row>
+    <row r="99" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B99" s="49"/>
+      <c r="C99" s="49"/>
+      <c r="D99" s="49"/>
+      <c r="E99" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="F99" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G99" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H99" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I99" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="J99" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K99" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="L99" s="22"/>
+    </row>
+    <row r="100" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B100" s="49"/>
+      <c r="C100" s="49"/>
+      <c r="D100" s="49"/>
+      <c r="E100" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="F100" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G100" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H100" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I100" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="J100" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K100" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="L100" s="22"/>
+    </row>
+    <row r="101" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B101" s="49"/>
+      <c r="C101" s="49"/>
+      <c r="D101" s="49"/>
+      <c r="E101" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="F101" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G101" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H101" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I101" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="J101" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K101" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="L101" s="22"/>
+    </row>
+    <row r="102" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B102" s="49"/>
+      <c r="C102" s="49"/>
+      <c r="D102" s="49"/>
+      <c r="E102" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="F102" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G102" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H102" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I102" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J102" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K102" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="L102" s="22"/>
+    </row>
+    <row r="103" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B103" s="49"/>
+      <c r="C103" s="49"/>
+      <c r="D103" s="49"/>
+      <c r="E103" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="F103" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G103" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H103" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I103" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="J103" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K103" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="L103" s="22"/>
+    </row>
+    <row r="104" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B104" s="49"/>
+      <c r="C104" s="49"/>
+      <c r="D104" s="49"/>
+      <c r="E104" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="F104" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G104" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H104" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I104" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="J104" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K104" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="L104" s="22"/>
+    </row>
+    <row r="105" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B105" s="49"/>
+      <c r="C105" s="49"/>
+      <c r="D105" s="49"/>
+      <c r="E105" s="30" t="s">
+        <v>274</v>
+      </c>
+      <c r="F105" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G105" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H105" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="I105" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="J105" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="K105" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="L105" s="22"/>
+    </row>
+    <row r="106" spans="1:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B106" s="49"/>
+      <c r="C106" s="49"/>
+      <c r="D106" s="49"/>
+      <c r="E106" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="F106" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G106" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H106" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="I106" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="J106" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="K106" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="L106" s="22"/>
+    </row>
+    <row r="107" spans="1:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B107" s="49"/>
+      <c r="C107" s="49"/>
+      <c r="D107" s="49"/>
+      <c r="E107" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G107" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H107" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="I107" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="J107" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K107" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="L107" s="22"/>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F108" s="56"/>
+      <c r="J108" s="57"/>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F109" s="56"/>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F110" s="56"/>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F111" s="56"/>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F112" s="56"/>
+    </row>
+    <row r="113" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F113" s="56"/>
+    </row>
+    <row r="114" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F114" s="56"/>
+    </row>
+    <row r="115" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F115" s="56"/>
+    </row>
+    <row r="116" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F116" s="56"/>
+    </row>
+    <row r="117" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F117" s="56"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="16">
+    <mergeCell ref="C81:C87"/>
+    <mergeCell ref="B81:B107"/>
+    <mergeCell ref="D81:D107"/>
+    <mergeCell ref="C89:C107"/>
+    <mergeCell ref="C9:C18"/>
+    <mergeCell ref="D9:D22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="B9:B22"/>
+    <mergeCell ref="C24:C32"/>
     <mergeCell ref="C59:C65"/>
     <mergeCell ref="C67:C79"/>
     <mergeCell ref="D59:D79"/>
@@ -3779,11 +4902,6 @@
     <mergeCell ref="C55:C57"/>
     <mergeCell ref="D24:D57"/>
     <mergeCell ref="C34:C53"/>
-    <mergeCell ref="C9:C18"/>
-    <mergeCell ref="D9:D22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="B9:B22"/>
-    <mergeCell ref="C24:C32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>